<commit_message>
Completed Verification of Yaxuan Inheritance Work.
</commit_message>
<xml_diff>
--- a/Project_Inheritance_Documentation/Image_processing_Details/Yaxuan_Li_Inheritance.xlsx
+++ b/Project_Inheritance_Documentation/Image_processing_Details/Yaxuan_Li_Inheritance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f337a85aa8871bf9/Desktop/japanese_project/japanese-handwriting-analysis/Project_Inheritance_Documentation/Image_processing_Details/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ANU\Semester_3\Advanced_Computing_Project\Project_Repo\japanese-handwriting-analysis\Project_Inheritance_Documentation\Image_Processing_Details\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{5299B244-BD3E-A04C-A35A-5A9B325FB1B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0964467C-A5CF-4548-865E-3117BDB716C5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2C9076-E7D5-4747-AC7D-0DFB71F13364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>How to Use It</t>
   </si>
@@ -110,28 +108,40 @@
     <t>Priority (if incomplete)</t>
   </si>
   <si>
-    <t>image preprocessing</t>
-  </si>
-  <si>
-    <t>done</t>
-  </si>
-  <si>
-    <t>No  already done</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
-    <t>google colab, use the code I pushed into the gitlab</t>
-  </si>
-  <si>
     <t>Image_processing/Copy_of_resized.ipynb</t>
   </si>
   <si>
-    <t>already handed over to Arslan</t>
-  </si>
-  <si>
     <t>Yes but image preprocessing part I think has already done.</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Image Preprocessing</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Google Colab, use the code I pushed into the gitlab</t>
+  </si>
+  <si>
+    <t>No,  already done</t>
+  </si>
+  <si>
+    <t>Already handed over to Muhammad Arslan</t>
+  </si>
+  <si>
+    <t>Yes, I have understood the task and it wasn't much complicated</t>
+  </si>
+  <si>
+    <t>Yes, the code runs in my system and I have installed all the required dependencies and installations and this part was not long, so it was easy to understand and inherit as well.</t>
+  </si>
+  <si>
+    <t>It's already completed as said to me by the members leaving the group members this semester but will als try to see if next semester we could come up with more efficient and good way for the Image PreProcessing Part.</t>
   </si>
 </sst>
 </file>
@@ -567,24 +577,27 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="78" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" customWidth="1"/>
-    <col min="6" max="6" width="39.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="41" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="21.46484375" customWidth="1"/>
-    <col min="10" max="10" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="32.796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="21.46484375" customWidth="1"/>
-    <col min="15" max="15" width="23" customWidth="1"/>
+    <col min="1" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="47.28515625" customWidth="1"/>
+    <col min="7" max="7" width="56.140625" customWidth="1"/>
+    <col min="8" max="9" width="21.42578125" customWidth="1"/>
+    <col min="10" max="10" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="39" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.42578125" customWidth="1"/>
+    <col min="13" max="13" width="58.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="159.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="200.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>18</v>
       </c>
@@ -605,7 +618,7 @@
       <c r="N1" s="9"/>
       <c r="O1" s="10"/>
     </row>
-    <row r="2" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -652,7 +665,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:15" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
@@ -683,7 +696,7 @@
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -691,36 +704,44 @@
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1" t="s">
+      <c r="I4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="M4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -737,7 +758,7 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -754,7 +775,7 @@
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -771,7 +792,7 @@
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -788,7 +809,7 @@
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -805,7 +826,7 @@
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -822,7 +843,7 @@
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -839,7 +860,7 @@
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -856,7 +877,7 @@
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -873,7 +894,7 @@
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -890,7 +911,7 @@
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -907,7 +928,7 @@
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -924,7 +945,7 @@
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -941,7 +962,7 @@
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -958,7 +979,7 @@
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -975,7 +996,7 @@
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -992,7 +1013,7 @@
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1009,7 +1030,7 @@
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1026,7 +1047,7 @@
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1043,7 +1064,7 @@
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1060,7 +1081,7 @@
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1077,7 +1098,7 @@
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1094,7 +1115,7 @@
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1111,7 +1132,7 @@
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1128,7 +1149,7 @@
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1145,7 +1166,7 @@
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1162,7 +1183,7 @@
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1179,7 +1200,7 @@
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1196,7 +1217,7 @@
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1213,7 +1234,7 @@
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1230,7 +1251,7 @@
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1247,7 +1268,7 @@
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1264,7 +1285,7 @@
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1281,7 +1302,7 @@
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1298,7 +1319,7 @@
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1315,7 +1336,7 @@
       <c r="N39" s="1"/>
       <c r="O39" s="1"/>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1332,7 +1353,7 @@
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1349,7 +1370,7 @@
       <c r="N41" s="1"/>
       <c r="O41" s="1"/>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>

</xml_diff>